<commit_message>
Updated the Responsibility Chart.
Updated what has been done as of the 12th of November, 2019.
</commit_message>
<xml_diff>
--- a/Responsibility Chart for ITWS Term Project.xlsx
+++ b/Responsibility Chart for ITWS Term Project.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dyerj\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dyerj\Documents\GitHub\Jam-Basket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31E8DAC-F746-48DD-948B-CF480A03667E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38F2944-02E7-44B0-839E-52327C6D8E28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{2297877C-F073-42A0-842F-3283DE0D4F66}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
   <si>
     <t>Responsibilities Chart for the ITWS Term Project</t>
   </si>
@@ -712,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CBEE96-9D72-4502-BFE3-BF2A89B281C5}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -797,7 +797,9 @@
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="13"/>
+      <c r="D7" s="13" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D8" s="13"/>
@@ -857,7 +859,9 @@
       <c r="C14" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="13"/>
+      <c r="D14" s="13" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -869,7 +873,9 @@
       <c r="C15" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="13"/>
+      <c r="D15" s="13" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1011,7 +1017,9 @@
       <c r="C29" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="13"/>
+      <c r="D29" s="13" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">

</xml_diff>